<commit_message>
Dash Hedge IPCA - 2026-02-08
</commit_message>
<xml_diff>
--- a/Dados/Ativos_Sem_Codigo.xlsx
+++ b/Dados/Ativos_Sem_Codigo.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
   <si>
     <t>Sub Classe</t>
   </si>
@@ -34,13 +34,16 @@
     <t>COD_XP</t>
   </si>
   <si>
-    <t>Debêntures</t>
-  </si>
-  <si>
-    <t>HAPV21</t>
-  </si>
-  <si>
-    <t>FIRF GERAES</t>
+    <t>CDB</t>
+  </si>
+  <si>
+    <t>CDB424EERW3</t>
+  </si>
+  <si>
+    <t>CDB3239C4TL</t>
+  </si>
+  <si>
+    <t>BBRASIL FIM</t>
   </si>
 </sst>
 </file>
@@ -402,7 +405,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -436,10 +439,24 @@
         <v>7</v>
       </c>
       <c r="C2" s="2">
-        <v>46213</v>
+        <v>46146</v>
       </c>
       <c r="D2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
         <v>8</v>
+      </c>
+      <c r="C3" s="2">
+        <v>46223</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>